<commit_message>
updated csv once more
</commit_message>
<xml_diff>
--- a/holds.xlsx
+++ b/holds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaden\Documents\github\KadenFranklin.github.io\rockwall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB09949D-B052-4656-819A-5E686717C328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5A4A38-FD3D-4049-AE21-BD9AD4E6CEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Hold pos. X</t>
-  </si>
-  <si>
-    <t>Hold pos. Y</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Hold ID?</t>
   </si>
@@ -43,6 +37,15 @@
   </si>
   <si>
     <t>[List of] routes</t>
+  </si>
+  <si>
+    <t>X-loc</t>
+  </si>
+  <si>
+    <t>Y-loc</t>
+  </si>
+  <si>
+    <t>spot-pos</t>
   </si>
 </sst>
 </file>
@@ -360,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,24 +378,27 @@
     <col min="5" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>